<commit_message>
Update on 2017-09-20, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,10 @@
   </si>
   <si>
     <t>保险水费班费(210+140+100)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,7 +419,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,6 +619,18 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12" s="1">
+        <v>42998</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">

</xml_diff>

<commit_message>
Update on 2017-09-25, 校园卡费用，76/月
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,14 @@
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校园卡费用（76/月）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,7 +427,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -636,6 +644,18 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>300</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43003</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">

</xml_diff>

<commit_message>
Updata on 2017-10-09, 收入生活费3000，支出生活费500
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,22 @@
   </si>
   <si>
     <t>校园卡费用（70/月）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(10/9~10/23)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,7 +443,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -661,10 +677,34 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43016</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43016</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Modified on 2017-10-13, 添加数据汇总信息
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2017年" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>生活费(10/9~10/23)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结余</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,16 +148,58 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -153,13 +207,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -440,327 +537,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.25" customWidth="1"/>
+    <col min="2" max="3" width="9" style="6"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.75" customWidth="1"/>
+    <col min="8" max="10" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="2:10" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="H2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="4">
         <v>19000</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E3" s="5">
         <v>42971</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="H3" s="8">
+        <f>SUMIFS(D3:D20001,C3:C20001,"收入")</f>
+        <v>22000</v>
+      </c>
+      <c r="I3" s="9">
+        <f>SUMIFS(D3:D20001,C3:C20001,"支出")</f>
+        <v>18970</v>
+      </c>
+      <c r="J3" s="10">
+        <f>H3-I3</f>
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
         <v>880</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="3">
         <v>42979</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
         <v>14000</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="3">
         <v>42979</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="C6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
         <v>1000</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E6" s="3">
         <v>42979</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
+      <c r="C7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
         <v>540</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="3">
         <v>42979</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
+      <c r="C8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
         <v>150</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E8" s="3">
         <v>42979</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2">
         <v>400</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E9" s="3">
         <v>42979</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="12">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
+      <c r="C10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E10" s="3">
         <v>42986</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="12">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
+      <c r="C11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
         <v>300</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E11" s="3">
         <v>42989</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="12">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
+      <c r="C12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
         <v>500</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E12" s="3">
         <v>42994</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
         <v>300</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E13" s="3">
         <v>42998</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="12">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="D14" s="2">
         <v>300</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E14" s="3">
         <v>43003</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="11">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14">
+      <c r="D15" s="4">
         <v>3000</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E15" s="5">
         <v>43016</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="12">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="D16" s="2">
         <v>500</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E16" s="3">
         <v>43016</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="C17" s="7"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="C18" s="7"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="7">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="C19" s="7"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="C20" s="7"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="C21" s="7"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="C22" s="7"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="C23" s="7"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="C24" s="7"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="C26" s="7"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="7">
         <v>25</v>
       </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Modified on 2017-10-13, 更新分类明细
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,31 +101,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(10/9~10/23)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结余</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>费用类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住宿费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其它</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>收入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生活费</t>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电脑费用5000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>支出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生活费(10/9~10/23)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总收入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总支出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结余</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -167,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +235,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -255,6 +301,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -537,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J27"/>
+  <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -548,13 +612,14 @@
     <col min="1" max="1" width="1.25" customWidth="1"/>
     <col min="2" max="3" width="9" style="6"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.75" customWidth="1"/>
-    <col min="8" max="10" width="9" style="6"/>
+    <col min="6" max="6" width="9.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.75" customWidth="1"/>
+    <col min="9" max="11" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -567,20 +632,23 @@
       <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="11">
         <v>1</v>
       </c>
@@ -593,23 +661,26 @@
       <c r="E3" s="5">
         <v>42971</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8">
-        <f>SUMIFS(D3:D20001,C3:C20001,"收入")</f>
-        <v>22000</v>
-      </c>
-      <c r="I3" s="9">
-        <f>SUMIFS(D3:D20001,C3:C20001,"支出")</f>
-        <v>18970</v>
-      </c>
-      <c r="J3" s="10">
-        <f>H3-I3</f>
+      <c r="I3" s="8">
+        <f>SUMIFS(D3:D20003,C3:C20003,"收入")</f>
+        <v>27000</v>
+      </c>
+      <c r="J3" s="9">
+        <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
+        <v>23970</v>
+      </c>
+      <c r="K3" s="10">
+        <f>I3-J3</f>
         <v>3030</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -622,11 +693,14 @@
       <c r="E4" s="3">
         <v>42979</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -639,11 +713,14 @@
       <c r="E5" s="3">
         <v>42979</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
         <v>4</v>
       </c>
@@ -656,11 +733,19 @@
       <c r="E6" s="3">
         <v>42979</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
         <v>5</v>
       </c>
@@ -673,11 +758,22 @@
       <c r="E7" s="3">
         <v>42979</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="19">
+        <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"学费")</f>
+        <v>14880</v>
+      </c>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
         <v>6</v>
       </c>
@@ -690,11 +786,22 @@
       <c r="E8" s="3">
         <v>42979</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="19">
+        <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"住宿费")</f>
+        <v>1540</v>
+      </c>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -707,11 +814,22 @@
       <c r="E9" s="3">
         <v>42979</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="19">
+        <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
+        <v>1500</v>
+      </c>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -724,11 +842,22 @@
       <c r="E10" s="3">
         <v>42986</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="19">
+        <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"其它")</f>
+        <v>6050</v>
+      </c>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -741,11 +870,14 @@
       <c r="E11" s="3">
         <v>42989</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="12">
         <v>10</v>
       </c>
@@ -758,11 +890,14 @@
       <c r="E12" s="3">
         <v>42994</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="12">
         <v>11</v>
       </c>
@@ -775,11 +910,14 @@
       <c r="E13" s="3">
         <v>42998</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -792,144 +930,211 @@
       <c r="E14" s="3">
         <v>43003</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="11">
         <v>13</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="E15" s="5">
-        <v>43016</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+        <v>43009</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="12">
         <v>14</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>43009</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="11">
+        <v>15</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43016</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="12">
+        <v>16</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
         <v>500</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="3">
         <v>43016</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="7">
-        <v>15</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="7">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="7">
         <v>17</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="7"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="7">
         <v>18</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="7"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7">
         <v>19</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="7"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="7">
         <v>20</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="7"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="7">
         <v>21</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="7"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7">
         <v>22</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="7"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7">
         <v>23</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="7"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="7">
         <v>24</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="7"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="7">
         <v>25</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="7">
+        <v>26</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="7">
+        <v>25</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Updata on 2017-10-23, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="2017年" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2017年'!$B$2:$G$29</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +169,14 @@
   </si>
   <si>
     <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(10/21~10/31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -272,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -312,10 +323,13 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -604,15 +618,16 @@
   <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.25" customWidth="1"/>
-    <col min="2" max="3" width="9" style="6"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.75" customWidth="1"/>
     <col min="9" max="11" width="9" style="6"/>
@@ -638,13 +653,13 @@
       <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -673,11 +688,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>23970</v>
+        <v>24270</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>3030</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -739,11 +754,11 @@
       <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
@@ -764,14 +779,14 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K7" s="19"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -792,14 +807,14 @@
       <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K8" s="19"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -820,14 +835,14 @@
       <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>1500</v>
-      </c>
-      <c r="K9" s="19"/>
+        <v>1800</v>
+      </c>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
@@ -848,14 +863,14 @@
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"其它")</f>
         <v>6050</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
@@ -1018,14 +1033,24 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="7">
+      <c r="B19" s="12">
         <v>17</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="1"/>
+      <c r="C19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2">
+        <v>300</v>
+      </c>
+      <c r="E19" s="3">
+        <v>43028</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="7">
@@ -1128,6 +1153,7 @@
       <c r="G29" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:G29"/>
   <mergeCells count="5">
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="J7:K7"/>

</xml_diff>

<commit_message>
Updata on 2017-10-23, 支出生活费20
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2017年'!$B$2:$G$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -177,6 +177,10 @@
   </si>
   <si>
     <t>生活费(10/21~10/31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -688,11 +692,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>24270</v>
+        <v>24290</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>2730</v>
+        <v>2710</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -840,7 +844,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>1800</v>
+        <v>1820</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1053,14 +1057,24 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="7">
+      <c r="B20" s="12">
         <v>18</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="1"/>
+      <c r="C20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
+        <v>43038</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7">

</xml_diff>

<commit_message>
Update on 2017-10-31, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2017年'!$B$2:$G$29</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(11/01-11/10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -621,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -692,11 +704,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>24290</v>
+        <v>24590</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>2710</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -844,7 +856,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>1820</v>
+        <v>2120</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1077,14 +1089,24 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="7">
+      <c r="B21" s="12">
         <v>19</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="1"/>
+      <c r="C21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2">
+        <v>300</v>
+      </c>
+      <c r="E21" s="3">
+        <v>43039</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="7">

</xml_diff>

<commit_message>
Update on 2017-11-09, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -180,19 +180,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>支出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生活费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>生活费(11/01-11/10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(11/11-11/20)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -634,7 +634,7 @@
   <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,11 +704,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>24590</v>
+        <v>24970</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>2410</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -856,7 +856,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>2120</v>
+        <v>2500</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1073,19 +1073,19 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="E20" s="3">
-        <v>43038</v>
+        <v>43039</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
@@ -1093,16 +1093,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2">
+        <v>400</v>
+      </c>
+      <c r="E21" s="3">
+        <v>43048</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" s="2">
-        <v>300</v>
-      </c>
-      <c r="E21" s="3">
-        <v>43039</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Update on 2017-11-09, 支出生活费300, 班费100
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>生活费(11/11-11/20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(11/21-11/30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -634,7 +646,7 @@
   <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,11 +716,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>24970</v>
+        <v>25370</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>2030</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -856,7 +868,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>2500</v>
+        <v>2800</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1109,24 +1121,44 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="7">
+      <c r="B22" s="12">
         <v>20</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="1"/>
+      <c r="C22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2">
+        <v>300</v>
+      </c>
+      <c r="E22" s="3">
+        <v>43060</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="7">
+      <c r="B23" s="12">
         <v>21</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="1"/>
+      <c r="C23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2">
+        <v>100</v>
+      </c>
+      <c r="E23" s="3">
+        <v>43060</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7">

</xml_diff>

<commit_message>
Update on 2017-11-29, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,6 +205,10 @@
   </si>
   <si>
     <t>班费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(12/01-12/10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -646,7 +650,7 @@
   <dimension ref="B1:K29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -716,11 +720,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>25370</v>
+        <v>25670</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>1630</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -868,7 +872,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>2800</v>
+        <v>3100</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1161,14 +1165,24 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="7">
+      <c r="B24" s="12">
         <v>22</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="1"/>
+      <c r="C24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="2">
+        <v>300</v>
+      </c>
+      <c r="E24" s="3">
+        <v>43060</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7">

</xml_diff>

<commit_message>
Update on 2017-12-22, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,6 +213,10 @@
   </si>
   <si>
     <t>生活费(12/11-12/20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(12/21-12/31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -653,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -724,11 +728,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>26070</v>
+        <v>26370</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>930</v>
+        <v>630</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -876,7 +880,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>3500</v>
+        <v>3800</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1209,14 +1213,24 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="7">
+      <c r="B26" s="12">
         <v>24</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="1"/>
+      <c r="C26" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2">
+        <v>300</v>
+      </c>
+      <c r="E26" s="3">
+        <v>43091</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="7">

</xml_diff>

<commit_message>
Update on 2018-1-2, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="2017年" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2017年'!$B$2:$G$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$B$2:$G$29</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,6 +217,10 @@
   </si>
   <si>
     <t>生活费(12/21-12/31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(1/1-1/10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -657,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -728,11 +732,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>26370</v>
+        <v>26670</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>630</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -880,7 +884,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>3800</v>
+        <v>4100</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1233,14 +1237,24 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="7">
+      <c r="B27" s="12">
         <v>25</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="1"/>
+      <c r="C27" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2">
+        <v>300</v>
+      </c>
+      <c r="E27" s="3">
+        <v>43102</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="7">

</xml_diff>

<commit_message>
Update on 2018-01-11, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,6 +221,10 @@
   </si>
   <si>
     <t>生活费(1/1-1/10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(1/11-放寒假)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -661,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -732,11 +736,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>26670</v>
+        <v>27070</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>330</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -884,7 +888,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>4100</v>
+        <v>4500</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1257,14 +1261,24 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="7">
+      <c r="B28" s="12">
         <v>26</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="1"/>
+      <c r="C28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2">
+        <v>400</v>
+      </c>
+      <c r="E28" s="3">
+        <v>43108</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="7">

</xml_diff>

<commit_message>
Update on 2018-03-06, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="第一学年" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$B$2:$G$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$2:$G$29</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,6 +225,10 @@
   </si>
   <si>
     <t>生活费(1/11-放寒假)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(3/6-3/15)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -663,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K29"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -736,11 +740,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>27070</v>
+        <v>27370</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>-70</v>
+        <v>-370</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -888,7 +892,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>4500</v>
+        <v>4800</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1281,14 +1285,134 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="7">
-        <v>25</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="1"/>
+      <c r="B29" s="12">
+        <v>27</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2">
+        <v>300</v>
+      </c>
+      <c r="E29" s="3">
+        <v>43165</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="12">
+        <v>28</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="12">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="12">
+        <v>30</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="12">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="12">
+        <v>32</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="12">
+        <v>33</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="12">
+        <v>34</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="12">
+        <v>35</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="12">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="12">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="12">
+        <v>38</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:G29"/>

</xml_diff>

<commit_message>
Update on 2018-03-16, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,10 @@
   </si>
   <si>
     <t>生活费(3/6-3/15)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(3/16-3/26)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,7 +674,7 @@
   <dimension ref="B1:K40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -740,11 +744,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>27370</v>
+        <v>27770</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>-370</v>
+        <v>-770</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -892,7 +896,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>4800</v>
+        <v>5200</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1308,11 +1312,21 @@
       <c r="B30" s="12">
         <v>28</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="1"/>
+      <c r="C30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2">
+        <v>400</v>
+      </c>
+      <c r="E30" s="3">
+        <v>43175</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="12">

</xml_diff>

<commit_message>
Update on 2018-04-11, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,6 +249,10 @@
   </si>
   <si>
     <t>生活费(司瀚生活费转)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(4/11-4/20)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -689,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -760,11 +764,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>28470</v>
+        <v>28770</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>1530</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -912,7 +916,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>5790</v>
+        <v>6090</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1428,11 +1432,21 @@
       <c r="B35" s="12">
         <v>33</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="1"/>
+      <c r="C35" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>300</v>
+      </c>
+      <c r="E35" s="3">
+        <v>43201</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="12">

</xml_diff>

<commit_message>
Update on 2018-04-24, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,6 +253,10 @@
   </si>
   <si>
     <t>生活费(4/11-4/20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(4/21-4/30)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -764,11 +768,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>28770</v>
+        <v>29170</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>1230</v>
+        <v>830</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -916,7 +920,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>6090</v>
+        <v>6490</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1452,11 +1456,21 @@
       <c r="B36" s="12">
         <v>34</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="1"/>
+      <c r="C36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2">
+        <v>400</v>
+      </c>
+      <c r="E36" s="3">
+        <v>43210</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="12">

</xml_diff>

<commit_message>
Update on 2018-04-30, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -257,6 +257,10 @@
   </si>
   <si>
     <t>生活费(4/21-4/30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(5/1-5/10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -697,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -768,11 +772,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>29170</v>
+        <v>29570</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>830</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -920,7 +924,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>6490</v>
+        <v>6890</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1476,11 +1480,21 @@
       <c r="B37" s="12">
         <v>35</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="1"/>
+      <c r="C37" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2">
+        <v>400</v>
+      </c>
+      <c r="E37" s="3">
+        <v>43220</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="12">

</xml_diff>

<commit_message>
Update on 2018-05-12, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -261,6 +261,10 @@
   </si>
   <si>
     <t>生活费(5/1-5/10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(5/11-5/20)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -701,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -772,11 +776,11 @@
       </c>
       <c r="J3" s="9">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>29570</v>
+        <v>29870</v>
       </c>
       <c r="K3" s="10">
         <f>I3-J3</f>
-        <v>430</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -924,7 +928,7 @@
       </c>
       <c r="J9" s="20">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>6890</v>
+        <v>7190</v>
       </c>
       <c r="K9" s="20"/>
     </row>
@@ -1500,11 +1504,21 @@
       <c r="B38" s="12">
         <v>36</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="1"/>
+      <c r="C38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2">
+        <v>300</v>
+      </c>
+      <c r="E38" s="3">
+        <v>43230</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="12">

</xml_diff>

<commit_message>
Update on 2018-05-21, 支出生活费400,班费100,其他100
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -265,6 +265,22 @@
   </si>
   <si>
     <t>生活费(5/11-5/20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班费100+拿药100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(5/21-5/31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -371,17 +387,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,842 +715,942 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K40"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.25" customWidth="1"/>
-    <col min="2" max="3" width="9.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.75" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.75" customWidth="1"/>
-    <col min="9" max="11" width="9" style="6"/>
+    <col min="9" max="11" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>19000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>42971</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <f>SUMIFS(D3:D20003,C3:C20003,"收入")</f>
         <v>30000</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>29870</v>
-      </c>
-      <c r="K3" s="10">
+        <v>30470</v>
+      </c>
+      <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>130</v>
+        <v>-470</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
         <v>880</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>42979</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
         <v>14000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>42979</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
         <v>1000</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>42979</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
         <v>540</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>42979</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
         <v>150</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>42979</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="12">
-        <v>7</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
         <v>400</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>42979</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>7190</v>
-      </c>
-      <c r="K9" s="20"/>
+        <v>7590</v>
+      </c>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1">
         <v>100</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>42986</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"其它")</f>
         <v>6050</v>
       </c>
-      <c r="K10" s="20"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
         <v>300</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>42989</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
         <v>500</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>42994</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
         <v>300</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>42998</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>12</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>300</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>43003</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>13</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>5000</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>43009</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="12">
+      <c r="B16" s="10">
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>5000</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>43009</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="11">
+      <c r="B17" s="9">
         <v>15</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>3000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>43016</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>500</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>43016</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="12">
+      <c r="B19" s="10">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>300</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>43028</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <v>18</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
         <v>300</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>43039</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <v>19</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>400</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>43048</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="12">
+      <c r="B22" s="10">
         <v>20</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1">
         <v>300</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>43060</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <v>21</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1">
         <v>100</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>43060</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <v>22</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
         <v>300</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>43060</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <v>23</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>400</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>43077</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <v>24</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>300</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>43091</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <v>25</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>300</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>43102</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>26</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
         <v>400</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>43108</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="12">
+      <c r="B29" s="10">
         <v>27</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
         <v>300</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>43165</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <v>28</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1">
         <v>400</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>43175</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="12">
+      <c r="B31" s="10">
         <v>29</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1">
         <v>190</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>43186</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="12">
+      <c r="B32" s="10">
         <v>30</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1">
         <v>110</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>43186</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="12">
+      <c r="B33" s="10">
         <v>31</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1">
         <v>400</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>43191</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="11">
+      <c r="B34" s="9">
         <v>32</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>3000</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>43196</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="12">
+      <c r="B35" s="10">
         <v>33</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="C35" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1">
         <v>300</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>43201</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="12">
+      <c r="B36" s="10">
         <v>34</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1">
         <v>400</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>43210</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="12">
+      <c r="B37" s="10">
         <v>35</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="C37" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1">
         <v>400</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>43220</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="12">
+      <c r="B38" s="10">
         <v>36</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1">
         <v>300</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>43230</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="12">
+      <c r="B39" s="10">
         <v>37</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="1"/>
+      <c r="C39" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1">
+        <v>200</v>
+      </c>
+      <c r="E39" s="2">
+        <v>43237</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="12">
+      <c r="B40" s="10">
         <v>38</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="1"/>
+      <c r="C40" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1">
+        <v>400</v>
+      </c>
+      <c r="E40" s="2">
+        <v>43241</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:G29"/>

</xml_diff>

<commit_message>
Update on 2018-05-30, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,6 +281,10 @@
   </si>
   <si>
     <t>生活费(5/21-5/31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(5/31-6/9)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -717,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -788,11 +792,11 @@
       </c>
       <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>30470</v>
+        <v>30770</v>
       </c>
       <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>-470</v>
+        <v>-770</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -940,7 +944,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>7590</v>
+        <v>7890</v>
       </c>
       <c r="K9" s="18"/>
     </row>
@@ -1573,12 +1577,24 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="B41" s="10">
+        <v>39</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1">
+        <v>300</v>
+      </c>
+      <c r="E41" s="2">
+        <v>43250</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="10"/>

</xml_diff>

<commit_message>
Update on 2018-06-10, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -285,6 +285,10 @@
   </si>
   <si>
     <t>生活费(5/31-6/9)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(6/10-6/19)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -721,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -792,11 +796,11 @@
       </c>
       <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>30770</v>
+        <v>31170</v>
       </c>
       <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>-770</v>
+        <v>-1170</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -944,7 +948,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>7890</v>
+        <v>8290</v>
       </c>
       <c r="K9" s="18"/>
     </row>
@@ -1584,7 +1588,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E41" s="2">
         <v>43250</v>
@@ -1597,12 +1601,24 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="B42" s="10">
+        <v>40</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1">
+        <v>300</v>
+      </c>
+      <c r="E42" s="2">
+        <v>43261</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="10"/>

</xml_diff>

<commit_message>
Update on 2018-06-29, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="1185"/>
   </bookViews>
   <sheets>
     <sheet name="第一学年" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -289,6 +289,10 @@
   </si>
   <si>
     <t>生活费(6/10-6/19)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(6/20-6/30)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -725,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -796,11 +800,11 @@
       </c>
       <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>31170</v>
+        <v>31570</v>
       </c>
       <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>-1170</v>
+        <v>-1570</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -948,7 +952,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>8290</v>
+        <v>8690</v>
       </c>
       <c r="K9" s="18"/>
     </row>
@@ -1621,12 +1625,24 @@
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="B43" s="10">
+        <v>41</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1">
+        <v>400</v>
+      </c>
+      <c r="E43" s="2">
+        <v>43270</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="10"/>

</xml_diff>

<commit_message>
Update on 2018-07-03, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -293,6 +293,10 @@
   </si>
   <si>
     <t>生活费(6/20-6/30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(7/1-7/10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -729,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -800,11 +804,11 @@
       </c>
       <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>31570</v>
+        <v>31970</v>
       </c>
       <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>-1570</v>
+        <v>-1970</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -952,7 +956,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>8690</v>
+        <v>9090</v>
       </c>
       <c r="K9" s="18"/>
     </row>
@@ -1645,12 +1649,24 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="B44" s="10">
+        <v>42</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1">
+        <v>400</v>
+      </c>
+      <c r="E44" s="2">
+        <v>43282</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="10"/>

</xml_diff>

<commit_message>
Update on 2018-07-10, 支出生活费100
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -10,7 +10,7 @@
     <sheet name="第一学年" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$2:$G$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$2:$G$45</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,10 +200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>其他</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>班费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -268,10 +264,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>其他</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>班费100+拿药100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -297,6 +289,10 @@
   </si>
   <si>
     <t>生活费(7/1-7/10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(7/11- )</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -733,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -804,11 +800,11 @@
       </c>
       <c r="J3" s="7">
         <f>SUMIFS(D3:D20003,C3:C20003,"支出")</f>
-        <v>31970</v>
+        <v>32070</v>
       </c>
       <c r="K3" s="8">
         <f>I3-J3</f>
-        <v>-1970</v>
+        <v>-2070</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -956,7 +952,7 @@
       </c>
       <c r="J9" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"生活费")</f>
-        <v>9090</v>
+        <v>9190</v>
       </c>
       <c r="K9" s="18"/>
     </row>
@@ -984,7 +980,7 @@
       </c>
       <c r="J10" s="18">
         <f>SUMIFS(D2:D20002,C2:C20002,"支出",F2:F20002,"其它")</f>
-        <v>6050</v>
+        <v>6460</v>
       </c>
       <c r="K10" s="18"/>
     </row>
@@ -1242,10 +1238,10 @@
         <v>43060</v>
       </c>
       <c r="F23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
@@ -1265,7 +1261,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -1285,7 +1281,7 @@
         <v>40</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1305,7 +1301,7 @@
         <v>40</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -1325,7 +1321,7 @@
         <v>40</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
@@ -1345,7 +1341,7 @@
         <v>15</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -1365,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -1385,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -1405,7 +1401,7 @@
         <v>15</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
@@ -1422,10 +1418,10 @@
         <v>43186</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -1445,7 +1441,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1465,7 +1461,7 @@
         <v>31</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -1485,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1505,7 +1501,7 @@
         <v>15</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1525,7 +1521,7 @@
         <v>15</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -1545,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -1562,10 +1558,10 @@
         <v>43237</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
@@ -1582,10 +1578,10 @@
         <v>43241</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -1605,7 +1601,7 @@
         <v>15</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -1625,7 +1621,7 @@
         <v>29</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
@@ -1645,7 +1641,7 @@
         <v>15</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
@@ -1665,16 +1661,28 @@
         <v>15</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="B45" s="10">
+        <v>43</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1">
+        <v>100</v>
+      </c>
+      <c r="E45" s="2">
+        <v>43291</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="10"/>
@@ -1717,7 +1725,7 @@
       <c r="G50" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G29"/>
+  <autoFilter ref="B2:G45"/>
   <mergeCells count="5">
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="J7:K7"/>

</xml_diff>

<commit_message>
Update on 2018-08-30, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="1185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="1185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="第一学年" sheetId="1" r:id="rId1"/>
+    <sheet name="第二学年" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">第二学年!$B$3:$G$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$3:$G$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,6 +299,26 @@
   </si>
   <si>
     <t>第一学年费用明细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租转生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一学年溢出生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二学年费用明细</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,14 +433,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -718,18 +750,18 @@
     <col min="9" max="11" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,8 +781,17 @@
         <v>4</v>
       </c>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -770,8 +811,20 @@
         <v>5</v>
       </c>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="10">
+        <f>SUMIFS(D4:D20000,C4:C20000,"收入")</f>
+        <v>30000</v>
+      </c>
+      <c r="J4" s="10">
+        <f>SUMIFS(D4:D20000,C4:C20000,"支出")</f>
+        <v>32070</v>
+      </c>
+      <c r="K4" s="10">
+        <f>I4-J4</f>
+        <v>-2070</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -791,8 +844,11 @@
         <v>8</v>
       </c>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -812,8 +868,11 @@
         <v>13</v>
       </c>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -833,8 +892,13 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -854,8 +918,16 @@
         <v>10</v>
       </c>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
+        <v>14880</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>6</v>
       </c>
@@ -875,8 +947,16 @@
         <v>11</v>
       </c>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
+        <v>1540</v>
+      </c>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
         <v>7</v>
       </c>
@@ -896,8 +976,16 @@
         <v>12</v>
       </c>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
+        <v>9190</v>
+      </c>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>8</v>
       </c>
@@ -917,8 +1005,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
+        <v>6460</v>
+      </c>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>9</v>
       </c>
@@ -938,8 +1034,9 @@
         <v>15</v>
       </c>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -960,7 +1057,7 @@
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
         <v>11</v>
       </c>
@@ -981,7 +1078,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="5">
         <v>12</v>
       </c>
@@ -1002,7 +1099,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
         <v>13</v>
       </c>
@@ -1671,119 +1768,55 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>24</v>
-      </c>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E49" s="4"/>
       <c r="F49" s="9"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="10">
-        <f ca="1">SUMIFS(D4:D20000,C4:C20000,"收入")</f>
-        <v>30000</v>
-      </c>
-      <c r="C50" s="10">
-        <f ca="1">SUMIFS(D4:D20000,C4:C20000,"支出")</f>
-        <v>32070</v>
-      </c>
-      <c r="D50" s="10">
-        <f ca="1">B50-C50</f>
-        <v>-2070</v>
-      </c>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E50" s="4"/>
       <c r="F50" s="9"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E51" s="4"/>
       <c r="F51" s="9"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E52" s="4"/>
       <c r="F52" s="9"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E53" s="4"/>
       <c r="F53" s="9"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="14">
-        <f ca="1">SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
-        <v>14880</v>
-      </c>
-      <c r="D54" s="14"/>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E54" s="4"/>
       <c r="F54" s="9"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C55" s="14">
-        <f ca="1">SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
-        <v>1540</v>
-      </c>
-      <c r="D55" s="14"/>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E55" s="4"/>
       <c r="F55" s="9"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="14">
-        <f ca="1">SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>9190</v>
-      </c>
-      <c r="D56" s="14"/>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E56" s="4"/>
       <c r="F56" s="9"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="14">
-        <f ca="1">SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
-        <v>6460</v>
-      </c>
-      <c r="D57" s="14"/>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E57" s="4"/>
       <c r="F57" s="9"/>
       <c r="G57" s="4"/>
@@ -1792,12 +1825,617 @@
   </sheetData>
   <autoFilter ref="B3:G46"/>
   <mergeCells count="6">
-    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K57"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.25" customWidth="1"/>
+    <col min="2" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.75" customWidth="1"/>
+    <col min="9" max="11" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6">
+        <f>6450+1850</f>
+        <v>8300</v>
+      </c>
+      <c r="E4" s="7">
+        <v>43342</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="10">
+        <f>SUMIFS(D4:D19989,C4:C19989,"收入")</f>
+        <v>8300</v>
+      </c>
+      <c r="J4" s="10">
+        <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
+        <v>2470</v>
+      </c>
+      <c r="K4" s="10">
+        <f>I4-J4</f>
+        <v>5830</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="16">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2070</v>
+      </c>
+      <c r="E5" s="7">
+        <v>43342</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>400</v>
+      </c>
+      <c r="E6" s="7">
+        <v>43342</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
+        <v>2470</v>
+      </c>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="13">
+        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B3:G46"/>
+  <mergeCells count="6">
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 2018-09-03, 收入生活费学费21800, 支出学费15900
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,10 +302,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>房租转生活费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -319,6 +315,38 @@
   </si>
   <si>
     <t>第二学年费用明细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费14000+住宿费1000+教材费700+保险200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租转生活费(2018年第2季度）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租转生活费(2018年第3季度）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,12 +397,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -404,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,17 +473,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -735,7 +773,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -751,14 +789,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -892,11 +930,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -921,11 +959,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -950,11 +988,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -979,11 +1017,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1008,11 +1046,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1843,7 +1881,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1853,20 +1891,20 @@
     <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.75" customWidth="1"/>
     <col min="9" max="11" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1917,40 +1955,40 @@
         <v>31</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"收入")</f>
-        <v>8300</v>
+        <v>30150</v>
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>2470</v>
+        <v>18370</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>5830</v>
+        <v>11780</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2070</v>
+      </c>
+      <c r="E5" s="16">
+        <v>43342</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="D5" s="17">
-        <v>2070</v>
-      </c>
-      <c r="E5" s="7">
-        <v>43342</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="9"/>
@@ -1971,10 +2009,10 @@
         <v>43342</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="9"/>
@@ -1982,52 +2020,88 @@
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E7" s="7">
+        <v>43346</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="12">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>43346</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="13"/>
+        <v>15900</v>
+      </c>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="12">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="6">
+        <v>15900</v>
+      </c>
+      <c r="E9" s="7">
+        <v>43346</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>0</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
@@ -2040,11 +2114,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>2470</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
@@ -2057,11 +2131,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="18">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>0</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
@@ -2430,12 +2504,12 @@
   </sheetData>
   <autoFilter ref="B3:G46"/>
   <mergeCells count="6">
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="B1:G1"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 2018-09-014, 支出生活费400,杂费390
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -347,6 +347,18 @@
   </si>
   <si>
     <t>房租转生活费(2018年第3季度）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其它</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补交住宿费200+车费50+水费140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,6 +492,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,14 +804,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -930,11 +945,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -959,11 +974,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -988,11 +1003,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1017,11 +1032,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1046,11 +1061,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="18"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1881,7 +1896,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1897,14 +1912,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1964,11 +1979,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>18370</v>
+        <v>19160</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>11780</v>
+        <v>10990</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2039,11 +2054,11 @@
         <v>80</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2068,11 +2083,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>15900</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2097,45 +2112,70 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>0</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="12">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
+        <v>400</v>
+      </c>
+      <c r="E10" s="7">
+        <v>43350</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>2470</v>
-      </c>
-      <c r="K10" s="18"/>
+        <v>2870</v>
+      </c>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <f>140+250</f>
+        <v>390</v>
+      </c>
+      <c r="E11" s="7">
+        <v>43357</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="19">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="18"/>
+        <v>390</v>
+      </c>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>

</xml_diff>

<commit_message>
Update on 2018-09-20, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -492,6 +492,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,14 +807,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -945,11 +948,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -974,11 +977,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="19"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1003,11 +1006,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="19"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1032,11 +1035,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1061,11 +1064,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="19"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1896,7 +1899,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1912,14 +1915,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1979,11 +1982,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>19160</v>
+        <v>19560</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>10990</v>
+        <v>10590</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2054,11 +2057,11 @@
         <v>80</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2083,11 +2086,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>15900</v>
       </c>
-      <c r="K8" s="19"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2112,11 +2115,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>0</v>
       </c>
-      <c r="K9" s="19"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
@@ -2141,11 +2144,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>2870</v>
-      </c>
-      <c r="K10" s="19"/>
+        <v>3270</v>
+      </c>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
@@ -2171,19 +2174,31 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>390</v>
       </c>
-      <c r="K11" s="19"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6">
+        <v>400</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43361</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2018-10-08, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -14,7 +14,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">第二学年!$B$3:$G$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$3:$G$46</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -359,6 +359,10 @@
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1899,7 +1903,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1982,11 +1986,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>19560</v>
+        <v>19960</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>10590</v>
+        <v>10190</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2146,7 +2150,7 @@
       </c>
       <c r="J10" s="20">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>3270</v>
+        <v>3670</v>
       </c>
       <c r="K10" s="20"/>
     </row>
@@ -2202,12 +2206,24 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="6">
+        <v>400</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43381</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2018-10-16, 支出生活费550
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="86">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -363,6 +363,10 @@
   </si>
   <si>
     <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-10-15 到 2018-10-31）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -454,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,6 +500,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -811,14 +818,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -952,11 +959,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -981,11 +988,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1010,11 +1017,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1039,11 +1046,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1068,11 +1075,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1903,7 +1910,7 @@
   <dimension ref="B1:K57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1919,14 +1926,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1986,11 +1993,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>19960</v>
+        <v>20510</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>10190</v>
+        <v>9640</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2061,11 +2068,11 @@
         <v>80</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2090,11 +2097,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>15900</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2119,11 +2126,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>0</v>
       </c>
-      <c r="K9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
@@ -2148,11 +2155,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>3670</v>
-      </c>
-      <c r="K10" s="20"/>
+        <v>4220</v>
+      </c>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
@@ -2178,11 +2185,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="21">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>390</v>
       </c>
-      <c r="K11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="12">
@@ -2227,12 +2234,24 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="12">
+        <v>11</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="6">
+        <v>550</v>
+      </c>
+      <c r="E14" s="7">
+        <v>43388</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2018-10-30, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -9,12 +9,13 @@
   <sheets>
     <sheet name="第一学年" sheetId="1" r:id="rId1"/>
     <sheet name="第二学年" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">第二学年!$B$3:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">第二学年!$B$3:$G$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$3:$G$46</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -338,10 +339,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>学费14000+住宿费1000+教材费700+保险200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>房租转生活费(2018年第2季度）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -354,10 +351,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>补交住宿费200+车费50+水费140</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -367,6 +360,33 @@
   </si>
   <si>
     <t>生活费(2018-10-15 到 2018-10-31）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-10-31 到 2018-11-9）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住宿费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补交住宿费200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车费50+水费140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费14000+教材费700+保险200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住宿费1000</t>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -458,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -513,11 +533,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,14 +847,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -959,11 +988,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -988,11 +1017,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="22">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1017,11 +1046,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="22">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1046,11 +1075,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="22">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1075,11 +1104,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="22">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1907,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K57"/>
+  <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1926,14 +1955,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1984,20 +2013,20 @@
         <v>31</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="10">
-        <f>SUMIFS(D4:D19989,C4:C19989,"收入")</f>
+        <f>SUMIFS(D4:D19991,C4:C19991,"收入")</f>
         <v>30150</v>
       </c>
       <c r="J4" s="10">
-        <f>SUMIFS(D4:D19989,C4:C19989,"支出")</f>
-        <v>20510</v>
+        <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
+        <v>20910</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>9640</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2065,14 +2094,14 @@
         <v>74</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2097,11 +2126,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="21">
-        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
-        <v>15900</v>
-      </c>
-      <c r="K8" s="21"/>
+      <c r="J8" s="22">
+        <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
+        <v>14900</v>
+      </c>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2111,7 +2140,7 @@
         <v>76</v>
       </c>
       <c r="D9" s="6">
-        <v>15900</v>
+        <v>14900</v>
       </c>
       <c r="E9" s="7">
         <v>43346</v>
@@ -2120,168 +2149,212 @@
         <v>77</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="21">
-        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="21"/>
+      <c r="J9" s="22">
+        <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
+        <v>1200</v>
+      </c>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
-        <v>7</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>7</v>
+      <c r="B10" s="21">
+        <v>7</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>76</v>
       </c>
       <c r="D10" s="6">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="7">
-        <v>43350</v>
+        <v>43346</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="21">
-        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
-        <v>4220</v>
-      </c>
-      <c r="K10" s="21"/>
+      <c r="J10" s="22">
+        <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
+        <v>4620</v>
+      </c>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="12">
+      <c r="B11" s="21">
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="6">
-        <f>140+250</f>
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="E11" s="7">
-        <v>43357</v>
+        <v>43350</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>81</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="21">
-        <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
-        <v>390</v>
-      </c>
-      <c r="K11" s="21"/>
+      <c r="J11" s="22">
+        <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
+        <v>190</v>
+      </c>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="12">
+      <c r="B12" s="21">
         <v>9</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6">
+        <v>190</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43357</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="21">
+        <v>10</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6">
+        <v>200</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43357</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="21">
+        <v>11</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6">
         <v>400</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E14" s="7">
         <v>43361</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="12">
-        <v>10</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="6">
-        <v>400</v>
-      </c>
-      <c r="E13" s="7">
-        <v>43381</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="12">
-        <v>11</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="6">
-        <v>550</v>
-      </c>
-      <c r="E14" s="7">
-        <v>43388</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="21">
+        <v>12</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="6">
+        <v>400</v>
+      </c>
+      <c r="E15" s="7">
+        <v>43381</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="21">
+        <v>13</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="6">
+        <v>550</v>
+      </c>
+      <c r="E16" s="7">
+        <v>43388</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="6"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="21">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="6">
+        <v>400</v>
+      </c>
+      <c r="E17" s="7">
+        <v>43403</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="6"/>
@@ -2289,8 +2362,11 @@
       <c r="F18" s="8"/>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="6"/>
@@ -2298,8 +2374,11 @@
       <c r="F19" s="8"/>
       <c r="G19" s="6"/>
       <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="6"/>
@@ -2307,8 +2386,11 @@
       <c r="F20" s="8"/>
       <c r="G20" s="6"/>
       <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="6"/>
@@ -2316,8 +2398,11 @@
       <c r="F21" s="8"/>
       <c r="G21" s="6"/>
       <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="6"/>
@@ -2325,8 +2410,11 @@
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
       <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="6"/>
@@ -2334,8 +2422,11 @@
       <c r="F23" s="8"/>
       <c r="G23" s="6"/>
       <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="6"/>
@@ -2343,8 +2434,11 @@
       <c r="F24" s="8"/>
       <c r="G24" s="6"/>
       <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="6"/>
@@ -2352,8 +2446,11 @@
       <c r="F25" s="8"/>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="6"/>
@@ -2361,8 +2458,11 @@
       <c r="F26" s="8"/>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="6"/>
@@ -2370,8 +2470,11 @@
       <c r="F27" s="8"/>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="6"/>
@@ -2379,8 +2482,11 @@
       <c r="F28" s="8"/>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="6"/>
@@ -2388,8 +2494,11 @@
       <c r="F29" s="8"/>
       <c r="G29" s="6"/>
       <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="6"/>
@@ -2397,8 +2506,11 @@
       <c r="F30" s="8"/>
       <c r="G30" s="6"/>
       <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="6"/>
@@ -2406,26 +2518,35 @@
       <c r="F31" s="8"/>
       <c r="G31" s="6"/>
       <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="6"/>
@@ -2433,62 +2554,83 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="6"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="6"/>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="8"/>
       <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="6"/>
+      <c r="G39" s="8"/>
       <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="6"/>
+      <c r="G40" s="8"/>
       <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="6"/>
@@ -2496,8 +2638,11 @@
       <c r="F41" s="8"/>
       <c r="G41" s="6"/>
       <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="6"/>
@@ -2505,8 +2650,11 @@
       <c r="F42" s="8"/>
       <c r="G42" s="6"/>
       <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="6"/>
@@ -2514,8 +2662,11 @@
       <c r="F43" s="8"/>
       <c r="G43" s="6"/>
       <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="6"/>
@@ -2523,8 +2674,11 @@
       <c r="F44" s="8"/>
       <c r="G44" s="6"/>
       <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="6"/>
@@ -2532,8 +2686,11 @@
       <c r="F45" s="8"/>
       <c r="G45" s="6"/>
       <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="6"/>
@@ -2541,58 +2698,115 @@
       <c r="F46" s="8"/>
       <c r="G46" s="6"/>
       <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="6"/>
       <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G48" s="4"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G49" s="4"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:G46"/>
+  <autoFilter ref="B3:G48"/>
   <mergeCells count="6">
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="B1:G1"/>
@@ -2605,4 +2819,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 2018-11-12, 支出生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="92">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,6 +387,10 @@
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-11-10 到 2018-11-19）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,17 +540,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,14 +854,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -988,11 +995,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1017,11 +1024,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="25">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1046,11 +1053,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="25">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1075,11 +1082,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="25">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1104,11 +1111,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="25">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1939,7 +1946,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1955,14 +1962,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2022,11 +2029,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>20910</v>
+        <v>21210</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>9240</v>
+        <v>8940</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2097,11 +2104,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2126,11 +2133,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="25">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2155,11 +2162,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="25">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2184,11 +2191,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="25">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>4620</v>
-      </c>
-      <c r="K10" s="22"/>
+        <v>4920</v>
+      </c>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2213,11 +2220,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="25">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>190</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2239,9 +2246,9 @@
         <v>87</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="21">
@@ -2355,12 +2362,24 @@
       <c r="K17"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="6"/>
+      <c r="B18" s="12">
+        <v>15</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="6">
+        <v>300</v>
+      </c>
+      <c r="E18" s="7">
+        <v>43414</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18"/>
       <c r="J18"/>

</xml_diff>

<commit_message>
Update on 2018-11-19, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="93">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -391,6 +391,10 @@
   </si>
   <si>
     <t>生活费(2018-11-10 到 2018-11-19）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-11-19 到 2018-11-30）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -482,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,6 +548,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -854,14 +861,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -995,11 +1002,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1024,11 +1031,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="26">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1053,11 +1060,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="26">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1082,11 +1089,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="26">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1111,11 +1118,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="26">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1946,7 +1953,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1962,14 +1969,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2029,11 +2036,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>21210</v>
+        <v>21610</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>8940</v>
+        <v>8540</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2104,11 +2111,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2133,11 +2140,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="26">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2162,11 +2169,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="26">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2191,11 +2198,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="26">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>4920</v>
-      </c>
-      <c r="K10" s="25"/>
+        <v>5320</v>
+      </c>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2220,11 +2227,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="26">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>190</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2386,12 +2393,24 @@
       <c r="K18"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="12">
+        <v>16</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6">
+        <v>400</v>
+      </c>
+      <c r="E19" s="7">
+        <v>43422</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19"/>
       <c r="J19"/>

</xml_diff>

<commit_message>
Update on 2018-11-29, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="94">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -363,10 +363,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生活费(2018-10-31 到 2018-11-9）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>住宿费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -395,6 +391,14 @@
   </si>
   <si>
     <t>生活费(2018-11-19 到 2018-11-30）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-11-29 到 2018-12-09）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-10-31 到 2018-11-09）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -548,6 +552,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -861,14 +868,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1002,11 +1009,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1031,11 +1038,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="27">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1060,11 +1067,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="27">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="26"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1089,11 +1096,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="27">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1118,11 +1125,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="27">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1953,7 +1960,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1969,14 +1976,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2036,11 +2043,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>21610</v>
+        <v>22010</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>8540</v>
+        <v>8140</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2111,11 +2118,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2140,11 +2147,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="27">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2163,17 +2170,17 @@
         <v>77</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="27">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="26"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2189,20 +2196,20 @@
         <v>43346</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="27">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>5320</v>
-      </c>
-      <c r="K10" s="26"/>
+        <v>5720</v>
+      </c>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2227,11 +2234,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="27">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>190</v>
       </c>
-      <c r="K11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2250,7 +2257,7 @@
         <v>80</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="23"/>
@@ -2271,10 +2278,10 @@
         <v>43357</v>
       </c>
       <c r="F13" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="H13" s="4"/>
     </row>
@@ -2313,7 +2320,7 @@
         <v>43381</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>15</v>
@@ -2361,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17"/>
@@ -2385,7 +2392,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18"/>
@@ -2409,7 +2416,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19"/>
@@ -2417,12 +2424,24 @@
       <c r="K19"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="6"/>
+      <c r="B20" s="12">
+        <v>17</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>400</v>
+      </c>
+      <c r="E20" s="7">
+        <v>43433</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20"/>
       <c r="J20"/>

</xml_diff>

<commit_message>
Update on 2018-12-10, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="95">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -399,6 +399,10 @@
   </si>
   <si>
     <t>生活费(2018-10-31 到 2018-11-09）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-12-10 到 2018-12-20）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,6 +556,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -868,14 +875,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1009,11 +1016,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1038,11 +1045,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="28">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1067,11 +1074,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="28">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1096,11 +1103,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="28">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1125,11 +1132,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="28">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1960,7 +1967,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1976,14 +1983,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2043,11 +2050,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>22010</v>
+        <v>22410</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>8140</v>
+        <v>7740</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2118,11 +2125,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2147,11 +2154,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="28">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2176,11 +2183,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="28">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2205,11 +2212,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="28">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>5720</v>
-      </c>
-      <c r="K10" s="27"/>
+        <v>6120</v>
+      </c>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2234,11 +2241,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="28">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>190</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2448,12 +2455,24 @@
       <c r="K20"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="6"/>
+      <c r="B21" s="27">
+        <v>18</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6">
+        <v>400</v>
+      </c>
+      <c r="E21" s="7">
+        <v>43444</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21"/>
       <c r="J21"/>

</xml_diff>

<commit_message>
Update on 2018-12-19, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,6 +403,14 @@
   </si>
   <si>
     <t>生活费(2018-12-10 到 2018-12-20）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2018-12-20 到 2018-12-31）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -858,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K57"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -1967,7 +1975,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2050,11 +2058,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>22410</v>
+        <v>22810</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>7740</v>
+        <v>7340</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2214,7 +2222,7 @@
       </c>
       <c r="J10" s="28">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>6120</v>
+        <v>6520</v>
       </c>
       <c r="K10" s="28"/>
     </row>
@@ -2479,12 +2487,24 @@
       <c r="K21"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="6"/>
+      <c r="B22" s="12">
+        <v>19</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="6">
+        <v>400</v>
+      </c>
+      <c r="E22" s="7">
+        <v>43453</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22"/>
       <c r="J22"/>

</xml_diff>

<commit_message>
Update on 2018-12-29, 支出生活费400
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="98">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -411,6 +411,10 @@
   </si>
   <si>
     <t>生活费(2018-12-20 到 2018-12-31）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-01-01 到 2019-01-09）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -502,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,6 +568,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -883,14 +890,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1024,11 +1031,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1053,11 +1060,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="29">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1082,11 +1089,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="29">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1111,11 +1118,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="29">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1140,11 +1147,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="29">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1974,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1991,14 +1998,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2058,11 +2065,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>22810</v>
+        <v>23210</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>7340</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2133,11 +2140,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2162,11 +2169,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="29">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2191,11 +2198,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="29">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2220,11 +2227,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="29">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>6520</v>
-      </c>
-      <c r="K10" s="28"/>
+        <v>6920</v>
+      </c>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2249,11 +2256,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="29">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>190</v>
       </c>
-      <c r="K11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2511,12 +2518,24 @@
       <c r="K22"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="6"/>
+      <c r="B23" s="12">
+        <v>20</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="6">
+        <v>400</v>
+      </c>
+      <c r="E23" s="7">
+        <v>43463</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23"/>
       <c r="J23"/>

</xml_diff>

<commit_message>
Update on 2019-01-09, 支出生活费400,期末聚餐费200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -415,6 +415,14 @@
   </si>
   <si>
     <t>生活费(2019-01-01 到 2019-01-09）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-01-10 到 放寒假）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放假聚餐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -506,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,6 +576,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,14 +901,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1031,11 +1042,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1060,11 +1071,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="30">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="29"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1089,11 +1100,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="30">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="29"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1118,11 +1129,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="30">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="29"/>
+      <c r="K10" s="30"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1147,11 +1158,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="30">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="29"/>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -1982,7 +1993,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1998,14 +2009,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2065,11 +2076,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>23210</v>
+        <v>23810</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>6940</v>
+        <v>6340</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2140,11 +2151,11 @@
         <v>79</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2169,11 +2180,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="30">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="29"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2198,11 +2209,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="30">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="29"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2227,11 +2238,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="30">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>6920</v>
-      </c>
-      <c r="K10" s="29"/>
+        <v>7320</v>
+      </c>
+      <c r="K10" s="30"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2256,11 +2267,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="30">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
-        <v>190</v>
-      </c>
-      <c r="K11" s="29"/>
+        <v>390</v>
+      </c>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2542,24 +2553,48 @@
       <c r="K23"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="6"/>
+      <c r="B24" s="29">
+        <v>21</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="6">
+        <v>400</v>
+      </c>
+      <c r="E24" s="7">
+        <v>43474</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
+      <c r="B25" s="29">
+        <v>22</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6">
+        <v>200</v>
+      </c>
+      <c r="E25" s="7">
+        <v>43481</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25"/>
       <c r="J25"/>

</xml_diff>

<commit_message>
Update on 2019-03-06, 支出生活费400+1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="106">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>房租转生活费(2019年第1季度）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-02-20 到 2019-02-28)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-03-01 到 2019-03-31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2005,7 +2017,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2088,11 +2100,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>23810</v>
+        <v>25410</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>12790</v>
+        <v>11190</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2252,7 +2264,7 @@
       </c>
       <c r="J10" s="30">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>7320</v>
+        <v>8920</v>
       </c>
       <c r="K10" s="30"/>
     </row>
@@ -2637,24 +2649,48 @@
       <c r="K26"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="6"/>
+      <c r="B27" s="12">
+        <v>24</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="6">
+        <v>400</v>
+      </c>
+      <c r="E27" s="7">
+        <v>43516</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="6"/>
+      <c r="B28" s="12">
+        <v>25</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E28" s="7">
+        <v>43527</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="H28" s="4"/>
       <c r="I28"/>
       <c r="J28"/>

</xml_diff>

<commit_message>
Update on 2019-04-06, 支出生活费1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="108">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -447,6 +447,14 @@
   </si>
   <si>
     <t>生活费(2019-03-01 到 2019-03-31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-04-01 到 2019-04-30)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2020,7 +2028,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2103,11 +2111,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>25410</v>
+        <v>26610</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>13040</v>
+        <v>11840</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2267,7 +2275,7 @@
       </c>
       <c r="J10" s="31">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>8920</v>
+        <v>10120</v>
       </c>
       <c r="K10" s="31"/>
     </row>
@@ -2724,12 +2732,24 @@
       <c r="K29"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="6"/>
+      <c r="B30" s="12">
+        <v>27</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E30" s="7">
+        <v>43554</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30"/>
       <c r="J30"/>

</xml_diff>

<commit_message>
Update on 2019-05-09, 支出生活费1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="109">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -455,6 +455,10 @@
   </si>
   <si>
     <t>生活费(2019-04-01 到 2019-04-30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-05-01 到 2019-05-31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,6 +612,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -936,14 +943,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1077,11 +1084,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1106,11 +1113,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="32">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="31"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1135,11 +1142,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="32">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="31"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1164,11 +1171,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="32">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="31"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1193,11 +1200,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="32">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -2027,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2044,14 +2051,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2111,11 +2118,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>26610</v>
+        <v>27810</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>11840</v>
+        <v>10640</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2186,11 +2193,11 @@
         <v>101</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2215,11 +2222,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="32">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="31"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2244,11 +2251,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="32">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="31"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2273,11 +2280,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="32">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>10120</v>
-      </c>
-      <c r="K10" s="31"/>
+        <v>11320</v>
+      </c>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2302,11 +2309,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="32">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>390</v>
       </c>
-      <c r="K11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2756,12 +2763,24 @@
       <c r="K30"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="6"/>
+      <c r="B31" s="12">
+        <v>28</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E31" s="7">
+        <v>43594</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="I31"/>
       <c r="J31"/>

</xml_diff>

<commit_message>
Update on 2019-06-02, 支出生活费1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="110">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -459,6 +459,10 @@
   </si>
   <si>
     <t>生活费(2019-05-01 到 2019-05-31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费(2019-06-01 到 2019-06-31)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -612,6 +616,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,14 +950,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1084,11 +1091,11 @@
         <v>9</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
@@ -1113,11 +1120,11 @@
       <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="33">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"学费")</f>
         <v>14880</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
@@ -1142,11 +1149,11 @@
       <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="33">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"住宿费")</f>
         <v>1540</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
@@ -1171,11 +1178,11 @@
       <c r="I10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="33">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"生活费")</f>
         <v>9190</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -1200,11 +1207,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="33">
         <f>SUMIFS(D3:D19999,C3:C19999,"支出",F3:F19999,"其它")</f>
         <v>6460</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
@@ -2035,7 +2042,7 @@
   <dimension ref="B1:K59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2051,14 +2058,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2118,11 +2125,11 @@
       </c>
       <c r="J4" s="10">
         <f>SUMIFS(D4:D19991,C4:C19991,"支出")</f>
-        <v>27810</v>
+        <v>29010</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>10640</v>
+        <v>9440</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -2193,11 +2200,11 @@
         <v>101</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
@@ -2222,11 +2229,11 @@
       <c r="I8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="33">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"学费")</f>
         <v>14900</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
@@ -2251,11 +2258,11 @@
       <c r="I9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="33">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"住宿费")</f>
         <v>1200</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
@@ -2280,11 +2287,11 @@
       <c r="I10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="33">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"生活费")</f>
-        <v>11320</v>
-      </c>
-      <c r="K10" s="32"/>
+        <v>12520</v>
+      </c>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
@@ -2309,11 +2316,11 @@
       <c r="I11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="33">
         <f>SUMIFS(D3:D20001,C3:C20001,"支出",F3:F20001,"其它")</f>
         <v>390</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
@@ -2787,12 +2794,24 @@
       <c r="K31"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="6"/>
+      <c r="B32" s="32">
+        <v>29</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E32" s="7">
+        <v>43618</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="H32" s="4"/>
       <c r="I32"/>
       <c r="J32"/>

</xml_diff>

<commit_message>
Update on 2019-08-27, 支出生活费1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="116">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -481,6 +481,14 @@
   </si>
   <si>
     <t>文泉房屋维修基金转生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3231,7 +3239,7 @@
   <dimension ref="B1:K65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3295,11 +3303,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D10:D19997,C10:C19997,"支出")</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>18143</v>
+        <v>16943</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3321,7 +3329,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"生活费")</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3407,11 +3415,21 @@
       <c r="B12" s="18">
         <v>3</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6"/>
+      <c r="C12" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43699</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2019-09-19, 更新学费，UI培训费用
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="122">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -480,15 +480,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文泉房屋维修基金转生活费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>支出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI培训班第一次培训费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费+住宿费等</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3239,7 +3263,7 @@
   <dimension ref="B1:K65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3294,20 +3318,20 @@
       </c>
       <c r="C4" s="24">
         <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"学费")</f>
-        <v>0</v>
+        <v>16120</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="10">
         <f>SUMIFS(D10:D19997,C10:C19997,"收入")</f>
-        <v>18143</v>
+        <v>25360</v>
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D10:D19997,C10:C19997,"支出")</f>
-        <v>1200</v>
+        <v>18320</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>16943</v>
+        <v>7040</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3370,44 +3394,44 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="18">
+      <c r="B10" s="12">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6">
-        <v>8903</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="C10" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="13">
+        <v>9240</v>
+      </c>
+      <c r="E10" s="14">
         <v>43670</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="12">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="13">
-        <v>9240</v>
-      </c>
-      <c r="E11" s="14">
-        <v>43670</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>112</v>
+      <c r="D11" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E11" s="7">
+        <v>43699</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -3416,19 +3440,19 @@
         <v>3</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D12" s="6">
-        <v>1200</v>
+        <v>16120</v>
       </c>
       <c r="E12" s="7">
-        <v>43699</v>
+        <v>43718</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H12" s="4"/>
     </row>
@@ -3436,22 +3460,42 @@
       <c r="B13" s="18">
         <v>4</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
+      <c r="C13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="6">
+        <v>16120</v>
+      </c>
+      <c r="E13" s="7">
+        <v>43718</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="18">
         <v>5</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
+      <c r="C14" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="7">
+        <v>43727</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
@@ -4061,7 +4105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Update on 2019-09-24, 更新房租
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">第二学年!$B$9:$G$54</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">第三学年!$B$9:$G$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">第三学年!$B$10:$G$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">第一学年!$B$9:$G$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="124">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -504,15 +504,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>UI培训班第一次培训费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学费+住宿费等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租（押一付六 * 600）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>培训费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI培训班第一次培训费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学费+住宿费等</t>
+    <t>培训费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -659,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,6 +735,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1035,14 +1046,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19"/>
@@ -1053,10 +1064,10 @@
       <c r="G2" s="19"/>
     </row>
     <row r="3" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="19"/>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -2185,14 +2196,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
@@ -2203,10 +2214,10 @@
       <c r="G2" s="19"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="25"/>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -3260,10 +3271,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K65"/>
+  <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3279,14 +3290,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
@@ -3297,10 +3308,10 @@
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="25"/>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -3317,21 +3328,21 @@
         <v>13</v>
       </c>
       <c r="C4" s="24">
-        <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"学费")</f>
+        <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"学费")</f>
         <v>16120</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="10">
-        <f>SUMIFS(D10:D19997,C10:C19997,"收入")</f>
+        <f>SUMIFS(D11:D19998,C11:C19998,"收入")</f>
         <v>25360</v>
       </c>
       <c r="F4" s="10">
-        <f>SUMIFS(D10:D19997,C10:C19997,"支出")</f>
-        <v>18320</v>
+        <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
+        <v>22520</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>7040</v>
+        <v>2840</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3339,7 +3350,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="24">
-        <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"住宿费")</f>
+        <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"住宿费")</f>
         <v>0</v>
       </c>
       <c r="D5" s="27"/>
@@ -3352,7 +3363,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="24">
-        <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"生活费")</f>
+        <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
         <v>1200</v>
       </c>
       <c r="D6" s="27"/>
@@ -3360,108 +3371,100 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="24">
+        <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"培训费")</f>
+        <v>5200</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="24">
-        <f>SUMIFS(D9:D20007,C9:C20007,"支出",F9:F20007,"其它")</f>
+      <c r="C8" s="24">
+        <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"其它")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="12">
         <v>1</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D11" s="13">
         <v>9240</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E11" s="14">
         <v>43670</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="F11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="18">
-        <v>2</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1200</v>
-      </c>
-      <c r="E11" s="7">
-        <v>43699</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D12" s="6">
-        <v>16120</v>
+        <v>1200</v>
       </c>
       <c r="E12" s="7">
-        <v>43718</v>
+        <v>43699</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D13" s="6">
         <v>16120</v>
@@ -3473,25 +3476,25 @@
         <v>116</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>118</v>
       </c>
       <c r="D14" s="6">
-        <v>1000</v>
+        <v>16120</v>
       </c>
       <c r="E14" s="7">
-        <v>43727</v>
+        <v>43718</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>120</v>
@@ -3500,29 +3503,49 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="18">
-        <v>6</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="7">
+        <v>43727</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="18">
-        <v>7</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="6">
+        <v>4200</v>
+      </c>
+      <c r="E16" s="7">
+        <v>43729</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="6"/>
@@ -3533,7 +3556,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="6"/>
@@ -3541,13 +3564,10 @@
       <c r="F18" s="8"/>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="6"/>
@@ -3555,10 +3575,13 @@
       <c r="F19" s="8"/>
       <c r="G19" s="6"/>
       <c r="H19" s="4"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="18">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="6"/>
@@ -3569,7 +3592,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="6"/>
@@ -3580,7 +3603,7 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="6"/>
@@ -3588,13 +3611,10 @@
       <c r="F22" s="8"/>
       <c r="G22" s="6"/>
       <c r="H22" s="4"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="18">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="6"/>
@@ -3608,7 +3628,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="6"/>
@@ -3622,7 +3642,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="6"/>
@@ -3636,7 +3656,7 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="6"/>
@@ -3650,7 +3670,7 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="6"/>
@@ -3664,7 +3684,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="18">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="6"/>
@@ -3678,7 +3698,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="6"/>
@@ -3692,7 +3712,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="6"/>
@@ -3706,7 +3726,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="18">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="6"/>
@@ -3720,7 +3740,7 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="18">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="6"/>
@@ -3734,7 +3754,7 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="18">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="6"/>
@@ -3748,7 +3768,7 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="6"/>
@@ -3762,7 +3782,7 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="18">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="6"/>
@@ -3776,7 +3796,7 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="18">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="6"/>
@@ -3790,7 +3810,7 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="18">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="6"/>
@@ -3804,7 +3824,7 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="18">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="6"/>
@@ -3818,7 +3838,7 @@
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="6"/>
@@ -3831,24 +3851,26 @@
       <c r="K39"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="18"/>
+      <c r="B40" s="18">
+        <v>30</v>
+      </c>
       <c r="C40" s="18"/>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="4"/>
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="H41" s="4"/>
       <c r="I41"/>
       <c r="J41"/>
@@ -3872,7 +3894,7 @@
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="F43" s="23"/>
-      <c r="G43" s="21"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="4"/>
       <c r="I43"/>
       <c r="J43"/>
@@ -3896,7 +3918,7 @@
       <c r="D45" s="21"/>
       <c r="E45" s="22"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="21"/>
       <c r="H45" s="4"/>
       <c r="I45"/>
       <c r="J45"/>
@@ -3920,7 +3942,7 @@
       <c r="D47" s="21"/>
       <c r="E47" s="22"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="21"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="4"/>
       <c r="I47"/>
       <c r="J47"/>
@@ -4013,17 +4035,22 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="4"/>
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G56" s="4"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
       <c r="H56" s="4"/>
       <c r="I56"/>
       <c r="J56"/>
@@ -4085,12 +4112,19 @@
       <c r="J64"/>
       <c r="K64"/>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+    </row>
+    <row r="66" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B9:G54"/>
+  <autoFilter ref="B10:G55"/>
   <mergeCells count="2">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Update on 2019-10-12, 更新生活费1200+300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="125">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -521,6 +521,10 @@
   </si>
   <si>
     <t>培训费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3273,8 +3277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3338,11 +3342,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>22520</v>
+        <v>24020</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>2840</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3364,7 +3368,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>1200</v>
+        <v>2700</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3547,22 +3551,42 @@
       <c r="B17" s="18">
         <v>7</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6">
+        <v>300</v>
+      </c>
+      <c r="E17" s="7">
+        <v>43735</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="18">
         <v>8</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="6"/>
+      <c r="C18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E18" s="7">
+        <v>43741</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2019-10-24, 更新生活费300
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="126">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3282,7 +3282,7 @@
   <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3346,11 +3346,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>24020</v>
+        <v>24320</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>1340</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>2700</v>
+        <v>3000</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3597,11 +3597,21 @@
       <c r="B19" s="18">
         <v>9</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="6"/>
+      <c r="C19" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6">
+        <v>300</v>
+      </c>
+      <c r="E19" s="7">
+        <v>43761</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="16"/>
       <c r="J19" s="17"/>

</xml_diff>

<commit_message>
Update on 2019-10-24, 更新生活费+培训费1500
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -529,6 +529,18 @@
   </si>
   <si>
     <t>第三学年费用明细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培训费按揭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2187,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3282,7 +3294,7 @@
   <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3346,11 +3358,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>24320</v>
+        <v>26020</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>1040</v>
+        <v>-660</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3372,7 +3384,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>3000</v>
+        <v>4390</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3385,7 +3397,7 @@
       </c>
       <c r="C7" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"培训费")</f>
-        <v>5200</v>
+        <v>5510</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="29"/>
@@ -3621,33 +3633,63 @@
       <c r="B20" s="18">
         <v>10</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="6"/>
+      <c r="C20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>200</v>
+      </c>
+      <c r="E20" s="7">
+        <v>43766</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="18">
         <v>11</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="6"/>
+      <c r="C21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6">
+        <v>110</v>
+      </c>
+      <c r="E21" s="7">
+        <v>43770</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="18">
         <v>12</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="6"/>
+      <c r="C22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1390</v>
+      </c>
+      <c r="E22" s="7">
+        <v>43770</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update on 2019-11-26, 更新生活费，指出600+200，收入9000
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="131">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -541,6 +541,14 @@
   </si>
   <si>
     <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欠妈的钱转生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3294,7 +3302,7 @@
   <dimension ref="B1:K66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3354,15 +3362,15 @@
       <c r="D4" s="26"/>
       <c r="E4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"收入")</f>
-        <v>25360</v>
+        <v>34360</v>
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>26020</v>
+        <v>26820</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>-660</v>
+        <v>7540</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3384,7 +3392,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>4390</v>
+        <v>5190</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3696,11 +3704,21 @@
       <c r="B23" s="18">
         <v>13</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="6"/>
+      <c r="C23" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6">
+        <v>600</v>
+      </c>
+      <c r="E23" s="7">
+        <v>43786</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -3710,11 +3728,21 @@
       <c r="B24" s="18">
         <v>14</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="6"/>
+      <c r="C24" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="6">
+        <v>200</v>
+      </c>
+      <c r="E24" s="7">
+        <v>43795</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -3724,11 +3752,21 @@
       <c r="B25" s="18">
         <v>15</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
+      <c r="C25" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="6">
+        <v>9000</v>
+      </c>
+      <c r="E25" s="7">
+        <v>43795</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25"/>
       <c r="J25"/>

</xml_diff>

<commit_message>
Update on 2019-11-26, 支出生活费1500
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="132">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -549,6 +549,10 @@
   </si>
   <si>
     <t>欠妈的钱转生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3301,7 +3305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -3366,11 +3370,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>26820</v>
+        <v>28320</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>7540</v>
+        <v>6040</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3392,7 +3396,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>5190</v>
+        <v>6690</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3776,11 +3780,21 @@
       <c r="B26" s="18">
         <v>16</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="6"/>
+      <c r="C26" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1500</v>
+      </c>
+      <c r="E26" s="7">
+        <v>43799</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26"/>
       <c r="J26"/>

</xml_diff>

<commit_message>
Update on 2019-12-31, 支出生活费1000
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="132">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3305,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3370,11 +3370,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>28320</v>
+        <v>29320</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>6040</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>6690</v>
+        <v>7690</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3804,11 +3804,21 @@
       <c r="B27" s="18">
         <v>17</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="6"/>
+      <c r="C27" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="7">
+        <v>43830</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H27" s="4"/>
       <c r="I27"/>
       <c r="J27"/>

</xml_diff>

<commit_message>
Update on 2020-03-11,　收入生活费1850
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="134">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -553,6 +553,14 @@
   </si>
   <si>
     <t>支出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租转生活费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2211,7 +2219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -3305,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3366,7 +3374,7 @@
       <c r="D4" s="26"/>
       <c r="E4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"收入")</f>
-        <v>34360</v>
+        <v>36210</v>
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
@@ -3374,7 +3382,7 @@
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>5040</v>
+        <v>6890</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3828,11 +3836,21 @@
       <c r="B28" s="18">
         <v>18</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="6"/>
+      <c r="C28" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E28" s="7">
+        <v>43899</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="H28" s="4"/>
       <c r="I28"/>
       <c r="J28"/>

</xml_diff>

<commit_message>
Update on 2020-03-25, 支出房租1200
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="136">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -561,6 +561,14 @@
   </si>
   <si>
     <t>房租转生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房租两个月</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3378,11 +3386,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>29320</v>
+        <v>31120</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>6890</v>
+        <v>5090</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3404,7 +3412,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>7690</v>
+        <v>8290</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3417,7 +3425,7 @@
       </c>
       <c r="C7" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"培训费")</f>
-        <v>5510</v>
+        <v>6710</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="29"/>
@@ -3860,11 +3868,21 @@
       <c r="B29" s="18">
         <v>19</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="6"/>
+      <c r="C29" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="6">
+        <v>600</v>
+      </c>
+      <c r="E29" s="7">
+        <v>43903</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -3874,11 +3892,21 @@
       <c r="B30" s="18">
         <v>20</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="6"/>
+      <c r="C30" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E30" s="7">
+        <v>43912</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="H30" s="4"/>
       <c r="I30"/>
       <c r="J30"/>

</xml_diff>

<commit_message>
Update on 2020-03-25, 支出生活费1０00
</commit_message>
<xml_diff>
--- a/WanHaoBillDetails.xlsx
+++ b/WanHaoBillDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="136">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1078,7 +1078,7 @@
   <dimension ref="B1:K63"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2227,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3321,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3386,11 +3386,11 @@
       </c>
       <c r="F4" s="10">
         <f>SUMIFS(D11:D19998,C11:C19998,"支出")</f>
-        <v>31120</v>
+        <v>32120</v>
       </c>
       <c r="G4" s="10">
         <f>E4-F4</f>
-        <v>5090</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3412,7 +3412,7 @@
       </c>
       <c r="C6" s="24">
         <f>SUMIFS(D10:D20008,C10:C20008,"支出",F10:F20008,"生活费")</f>
-        <v>8290</v>
+        <v>9290</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="29"/>
@@ -3916,11 +3916,21 @@
       <c r="B31" s="18">
         <v>21</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="6"/>
+      <c r="C31" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E31" s="7">
+        <v>43922</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H31" s="4"/>
       <c r="I31"/>
       <c r="J31"/>

</xml_diff>